<commit_message>
Excel File upload done
</commit_message>
<xml_diff>
--- a/EasyAssetManager/wwwroot/UserSpace/ISHTIAQUE01/LOAN_PORTFOLIO.xlsx
+++ b/EasyAssetManager/wwwroot/UserSpace/ISHTIAQUE01/LOAN_PORTFOLIO.xlsx
@@ -22,15 +22,6 @@
     <t>CTG 2</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>195</t>
   </si>
   <si>
@@ -68,6 +59,15 @@
   </si>
   <si>
     <t>Loan_Acct_No</t>
+  </si>
+  <si>
+    <t>Sayful</t>
+  </si>
+  <si>
+    <t>Suman</t>
+  </si>
+  <si>
+    <t>Hasinul</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,25 +537,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -563,22 +563,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" s="7">
         <v>1222</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -589,19 +589,19 @@
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E3" s="7">
         <v>1290</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -612,19 +612,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E4" s="7">
         <v>2003</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>